<commit_message>
build: adicionar minha CI
</commit_message>
<xml_diff>
--- a/data/contrato_errado.xlsx
+++ b/data/contrato_errado.xlsx
@@ -50,17 +50,25 @@
     <t>categoria1</t>
   </si>
   <si>
-    <t>mateus</t>
+    <t>mateus@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,14 +91,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -372,7 +383,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,7 +415,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1">
@@ -417,7 +428,7 @@
         <v>6</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -425,7 +436,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="joao@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>